<commit_message>
[Added] Filas errores excel
</commit_message>
<xml_diff>
--- a/formatos/Productos vs Materia prima.xlsx
+++ b/formatos/Productos vs Materia prima.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desarrollo\Tezlik\htdocs\formatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\desarrollo\Tezlik\htdocs\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE484F73-B8F8-47CD-B39F-BBDDF13D7873}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED3C9CA-4A28-4630-8C51-98FDAFC1DAF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Configuracion productos" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Referencia</t>
-  </si>
-  <si>
-    <t>Producto</t>
   </si>
   <si>
     <t>Material</t>
@@ -424,19 +421,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.875" customWidth="1"/>
-    <col min="2" max="2" width="35.375" customWidth="1"/>
-    <col min="3" max="3" width="40" customWidth="1"/>
-    <col min="4" max="4" width="18.875" customWidth="1"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
+    <col min="3" max="3" width="18.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,27 +444,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:D1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1 B1:C1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>